<commit_message>
Mise en place de la communication can, avec vérification du bon acquitement et des mouvement. Il manque la mise en place de la fonction xytheta et du recalage
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125B88E7-0640-4080-BFA8-3866B6E24FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD44A7-4CBF-4F82-953A-F33758F5302D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16392" yWindow="0" windowWidth="6744" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hex_Dec_Bin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -72,6 +73,12 @@
   </si>
   <si>
     <t>Consigne dist d</t>
+  </si>
+  <si>
+    <t>Décimal</t>
+  </si>
+  <si>
+    <t>Hexadécimal</t>
   </si>
 </sst>
 </file>
@@ -391,7 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -529,4 +536,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB51A4F7-7582-4569-A88C-DC61C5905402}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="str">
+        <f>DEC2HEX(B2)</f>
+        <v>FFFFFFFFFF</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PROBLEME DIRECTION EFFECTUER TOUT FONCTIONNE IL FAUT QUE REGLER PROBLEME ROUE ODOO XYTHETA ET RECALAGE
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD44A7-4CBF-4F82-953A-F33758F5302D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125B88E7-0640-4080-BFA8-3866B6E24FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16392" yWindow="0" windowWidth="6744" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hex_Dec_Bin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -73,12 +72,6 @@
   </si>
   <si>
     <t>Consigne dist d</t>
-  </si>
-  <si>
-    <t>Décimal</t>
-  </si>
-  <si>
-    <t>Hexadécimal</t>
   </si>
 </sst>
 </file>
@@ -398,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -536,36 +529,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB51A4F7-7582-4569-A88C-DC61C5905402}">
-  <dimension ref="A2:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="str">
-        <f>DEC2HEX(B2)</f>
-        <v>FFFFFFFFFF</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Mise en place du freinage fonctionnelle, maintenant il faut régler la rotation et la dérive quand on avance
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125B88E7-0640-4080-BFA8-3866B6E24FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE0BD88-56F5-47E1-87C6-EFE440AED096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16392" yWindow="0" windowWidth="6744" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I22"/>
+  <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,6 +526,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <f>A25*B24/A24</f>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Freinage et calcul de la rotation fonctionnelle ainsi que la ligne droite, on observe une dérive non négligeable
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE0BD88-56F5-47E1-87C6-EFE440AED096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F47F251-82FF-432C-963A-5E77F4A03465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -53,25 +53,37 @@
     <t>Odo finaux</t>
   </si>
   <si>
-    <t>Consigne vit gauche</t>
-  </si>
-  <si>
-    <t>Offset</t>
-  </si>
-  <si>
-    <t>Consigne dist gauche</t>
-  </si>
-  <si>
-    <t>Xconsigne_dist_gauche 3406</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Xconsigne_vit_gauche -120</t>
-  </si>
-  <si>
-    <t>Odo</t>
-  </si>
-  <si>
-    <t>Consigne dist d</t>
+    <t>Angle cons</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Pour</t>
+  </si>
+  <si>
+    <t>Largeur du robot</t>
+  </si>
+  <si>
+    <t>Distance qu'il va parcourir</t>
+  </si>
+  <si>
+    <t>Conversion en tick</t>
+  </si>
+  <si>
+    <t>Size whell diameter</t>
+  </si>
+  <si>
+    <t>Résolution roue codeus</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>Périmètre cercle avec D = Largeur du robot</t>
   </si>
 </sst>
 </file>
@@ -87,15 +99,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,12 +133,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,18 +464,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I25"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -410,16 +491,67 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>50</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2">
+        <v>50</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>5000</v>
       </c>
       <c r="C3">
         <v>5000</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2">
+        <v>50</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2048</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2048</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="K4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="2">
+        <v>80</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -430,8 +562,36 @@
         <f>-B5</f>
         <v>-2250</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2">
+        <v>250</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="5">
+        <f>L2*L3/L4</f>
+        <v>1280</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2">
+        <f>PI()*H5</f>
+        <v>785.39816339744823</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -443,106 +603,28 @@
         <f>C5+C3</f>
         <v>2750</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="2">
+        <f>H6*H2/360</f>
+        <v>109.08307824964558</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="8" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>4310</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13">
-        <v>3406</v>
-      </c>
-      <c r="H13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13">
-        <v>4730</v>
-      </c>
+      <c r="H8" s="5">
+        <f>H7*(H4/(2*PI()*H3/2))</f>
+        <v>1422.2222222222219</v>
+      </c>
+      <c r="I8" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14">
-        <v>-120</v>
-      </c>
-      <c r="H14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>510</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <f>F13-F14*5</f>
-        <v>4006</v>
-      </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15">
-        <f>I13-I14*5</f>
-        <v>5330</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <f>B13+(B15)*5</f>
-        <v>6860</v>
-      </c>
-      <c r="F17">
-        <f>F15+F14*5</f>
-        <v>3406</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>10</v>
-      </c>
-      <c r="B24">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>20</v>
-      </c>
-      <c r="B25">
-        <f>A25*B24/A24</f>
-        <v>3</v>
-      </c>
-    </row>
+    <row r="9" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rectification calcul rotation +petit commentaire + effacement commentaire
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F47F251-82FF-432C-963A-5E77F4A03465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BF4222-2FC8-4A39-84AE-A1967D6C7BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="2">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>14</v>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="2">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>14</v>
@@ -566,7 +566,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="2">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>13</v>
@@ -576,7 +576,7 @@
       </c>
       <c r="L5" s="5">
         <f>L2*L3/L4</f>
-        <v>1280</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -585,7 +585,7 @@
       </c>
       <c r="H6" s="2">
         <f>PI()*H5</f>
-        <v>785.39816339744823</v>
+        <v>706.85834705770344</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>13</v>
@@ -608,7 +608,7 @@
       </c>
       <c r="H7" s="2">
         <f>H6*H2/360</f>
-        <v>109.08307824964558</v>
+        <v>176.71458676442586</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>13</v>
@@ -620,7 +620,7 @@
       </c>
       <c r="H8" s="5">
         <f>H7*(H4/(2*PI()*H3/2))</f>
-        <v>1422.2222222222219</v>
+        <v>2304</v>
       </c>
       <c r="I8" s="1"/>
     </row>

</xml_diff>

<commit_message>
Mise en place du mouvement x y theta, a régler probleme de précision
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BF4222-2FC8-4A39-84AE-A1967D6C7BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B81951-A6D4-4444-85D0-5E251D4669D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -84,12 +84,52 @@
   </si>
   <si>
     <t>Périmètre cercle avec D = Largeur du robot</t>
+  </si>
+  <si>
+    <t>coordonne x</t>
+  </si>
+  <si>
+    <t>coordonne y</t>
+  </si>
+  <si>
+    <t>theta fin</t>
+  </si>
+  <si>
+    <t>Hypothenuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theta rot </t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>Theta fin rotation</t>
+  </si>
+  <si>
+    <t>Calcul x y theta</t>
+  </si>
+  <si>
+    <t>Delta de ce que j'ai</t>
+  </si>
+  <si>
+    <t>Ce que j'obtiens</t>
+  </si>
+  <si>
+    <t>Pourcentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +161,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,6 +228,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,24 +524,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -510,7 +571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>5000</v>
       </c>
@@ -533,7 +594,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
@@ -551,7 +612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -579,7 +640,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
@@ -591,7 +652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -614,7 +675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G8" s="4" t="s">
         <v>10</v>
       </c>
@@ -624,7 +685,149 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14">
+        <f>3/640</f>
+        <v>4.6874999999999998E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="2">
+        <v>100</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="1">
+        <v>101</v>
+      </c>
+      <c r="L15" s="13">
+        <f>K15/H15</f>
+        <v>1.01</v>
+      </c>
+      <c r="M15" s="12">
+        <f>(1-L15)*100</f>
+        <v>-1.0000000000000009</v>
+      </c>
+      <c r="P15">
+        <f>P14*100</f>
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="2">
+        <v>100</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="1">
+        <v>101</v>
+      </c>
+      <c r="L16" s="13">
+        <f t="shared" ref="L16:L17" si="0">K16/H16</f>
+        <v>1.01</v>
+      </c>
+      <c r="M16" s="12">
+        <f t="shared" ref="M16:M17" si="1">(1-L16)*100</f>
+        <v>-1.0000000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="2">
+        <v>90</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="1">
+        <v>99</v>
+      </c>
+      <c r="L17" s="13">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M17" s="12">
+        <f t="shared" si="1"/>
+        <v>-10.000000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="10">
+        <f>SQRT(H15*H15+H16*H16)</f>
+        <v>141.42135623730951</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="11">
+        <f>ATAN2(H15,H16)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="8"/>
+      <c r="H21" s="10">
+        <f>DEGREES(H20)</f>
+        <v>45</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="10">
+        <f>H17-H21</f>
+        <v>45</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="7:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Le freinage admet toujours des a coup mais je n'y arrive pas a faire mieux.
Concernant le niveau de précision j'arrive au max a etre 1.5%

Globalement le programme peut etre utilisé lors de la coupe dans cet etat avec le mode de vitesse TORTUE
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B81951-A6D4-4444-85D0-5E251D4669D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C47C51-5564-4F53-8DEA-C2EB607F060F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Pourcentage</t>
+  </si>
+  <si>
+    <t>Tension alim avec test</t>
+  </si>
+  <si>
+    <t>Tension en cours</t>
+  </si>
+  <si>
+    <t>Coeff en</t>
   </si>
 </sst>
 </file>
@@ -526,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,7 +615,7 @@
         <v>7</v>
       </c>
       <c r="L4" s="2">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>14</v>
@@ -627,7 +636,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="2">
-        <v>225</v>
+        <v>193.55</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>13</v>
@@ -637,7 +646,7 @@
       </c>
       <c r="L5" s="5">
         <f>L2*L3/L4</f>
-        <v>2304</v>
+        <v>1981.9354838709678</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -646,7 +655,7 @@
       </c>
       <c r="H6" s="2">
         <f>PI()*H5</f>
-        <v>706.85834705770344</v>
+        <v>608.05525810230449</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>13</v>
@@ -669,7 +678,7 @@
       </c>
       <c r="H7" s="2">
         <f>H6*H2/360</f>
-        <v>176.71458676442586</v>
+        <v>152.01381452557612</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>13</v>
@@ -681,13 +690,35 @@
       </c>
       <c r="H8" s="5">
         <f>H7*(H4/(2*PI()*H3/2))</f>
-        <v>2304</v>
+        <v>1981.952</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
     <row r="14" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <f>B12/B13</f>
+        <v>1.3</v>
+      </c>
       <c r="G14" s="9" t="s">
         <v>24</v>
       </c>
@@ -716,15 +747,15 @@
         <v>13</v>
       </c>
       <c r="K15" s="1">
-        <v>101</v>
+        <v>100.28</v>
       </c>
       <c r="L15" s="13">
         <f>K15/H15</f>
-        <v>1.01</v>
+        <v>1.0027999999999999</v>
       </c>
       <c r="M15" s="12">
         <f>(1-L15)*100</f>
-        <v>-1.0000000000000009</v>
+        <v>-0.27999999999999137</v>
       </c>
       <c r="P15">
         <f>P14*100</f>
@@ -742,15 +773,15 @@
         <v>13</v>
       </c>
       <c r="K16" s="1">
-        <v>101</v>
+        <v>101.26900000000001</v>
       </c>
       <c r="L16" s="13">
         <f t="shared" ref="L16:L17" si="0">K16/H16</f>
-        <v>1.01</v>
+        <v>1.0126900000000001</v>
       </c>
       <c r="M16" s="12">
         <f t="shared" ref="M16:M17" si="1">(1-L16)*100</f>
-        <v>-1.0000000000000009</v>
+        <v>-1.269000000000009</v>
       </c>
     </row>
     <row r="17" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -764,15 +795,15 @@
         <v>22</v>
       </c>
       <c r="K17" s="1">
-        <v>99</v>
+        <v>90.09</v>
       </c>
       <c r="L17" s="13">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>1.0010000000000001</v>
       </c>
       <c r="M17" s="12">
         <f t="shared" si="1"/>
-        <v>-10.000000000000009</v>
+        <v>-0.10000000000001119</v>
       </c>
     </row>
     <row r="18" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
La fonction xytheta fonctionne mais entre le faire depuis la base ou depuis des commande individuelle, je ne vois pas trop de difference
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C47C51-5564-4F53-8DEA-C2EB607F060F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7260B485-0804-4A92-9678-CD960D715E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,7 +789,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>22</v>
@@ -797,13 +797,13 @@
       <c r="K17" s="1">
         <v>90.09</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>1.0010000000000001</v>
-      </c>
-      <c r="M17" s="12">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>-0.10000000000001119</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -852,7 +852,7 @@
       </c>
       <c r="H23" s="10">
         <f>H17-H21</f>
-        <v>45</v>
+        <v>-45</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Quand je fais une rotation de 360 degres, je dévie seulement de 0.2mm en x et en y.
La maniere dont cela a été fait est totalement est bon car au fait le probleme vient du fait de la maniere dont je gère la vitesse.

Le code est bon dans sa globalité, il faut mtn passer au nettoyage en retirant toutes les variable qui ne serve a rien (de l'ordre d'une dizaine)
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7260B485-0804-4A92-9678-CD960D715E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EE28C4-534F-4266-B3AC-08B1BFBCA12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -129,6 +129,21 @@
   </si>
   <si>
     <t>Coeff en</t>
+  </si>
+  <si>
+    <t>consigne rot gauche</t>
+  </si>
+  <si>
+    <t>consigne rot droite</t>
+  </si>
+  <si>
+    <t>Vcc</t>
+  </si>
+  <si>
+    <t>Consigne gauche cc</t>
+  </si>
+  <si>
+    <t>Consigne droite cc</t>
   </si>
 </sst>
 </file>
@@ -533,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +756,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="2">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>13</v>
@@ -751,11 +766,11 @@
       </c>
       <c r="L15" s="13">
         <f>K15/H15</f>
-        <v>1.0027999999999999</v>
+        <v>1.5917460317460317</v>
       </c>
       <c r="M15" s="12">
         <f>(1-L15)*100</f>
-        <v>-0.27999999999999137</v>
+        <v>-59.17460317460317</v>
       </c>
       <c r="P15">
         <f>P14*100</f>
@@ -767,7 +782,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="2">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>13</v>
@@ -777,11 +792,11 @@
       </c>
       <c r="L16" s="13">
         <f t="shared" ref="L16:L17" si="0">K16/H16</f>
-        <v>1.0126900000000001</v>
+        <v>1.7164237288135593</v>
       </c>
       <c r="M16" s="12">
         <f t="shared" ref="M16:M17" si="1">(1-L16)*100</f>
-        <v>-1.269000000000009</v>
+        <v>-71.642372881355925</v>
       </c>
     </row>
     <row r="17" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -789,7 +804,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>22</v>
@@ -797,13 +812,13 @@
       <c r="K17" s="1">
         <v>90.09</v>
       </c>
-      <c r="L17" s="13" t="e">
+      <c r="L17" s="13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" s="12" t="e">
+        <v>0.99</v>
+      </c>
+      <c r="M17" s="12">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.0000000000000009</v>
       </c>
     </row>
     <row r="18" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -815,7 +830,7 @@
       </c>
       <c r="H19" s="10">
         <f>SQRT(H15*H15+H16*H16)</f>
-        <v>141.42135623730951</v>
+        <v>86.313382508160345</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>13</v>
@@ -827,7 +842,7 @@
       </c>
       <c r="H20" s="11">
         <f>ATAN2(H15,H16)</f>
-        <v>0.78539816339744828</v>
+        <v>0.75262301899337258</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>21</v>
@@ -837,7 +852,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="10">
         <f>DEGREES(H20)</f>
-        <v>45</v>
+        <v>43.122122552714643</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>22</v>
@@ -852,13 +867,56 @@
       </c>
       <c r="H23" s="10">
         <f>H17-H21</f>
-        <v>-45</v>
+        <v>47.877877447285357</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="7:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26">
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="27" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="28" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28">
+        <f>(($H$26)-($H$27))/2</f>
+        <v>59.75</v>
+      </c>
+    </row>
+    <row r="29" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29">
+        <f>H28</f>
+        <v>59.75</v>
+      </c>
+    </row>
+    <row r="30" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30">
+        <f>-H28</f>
+        <v>-59.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise au propre d'une grande partie du code et clarification a quelques endroit
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EE28C4-534F-4266-B3AC-08B1BFBCA12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7CF3F0-1B76-45A0-B2DF-1B15E9650236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +756,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="2">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>13</v>
@@ -766,11 +766,11 @@
       </c>
       <c r="L15" s="13">
         <f>K15/H15</f>
-        <v>1.5917460317460317</v>
+        <v>1.1142222222222222</v>
       </c>
       <c r="M15" s="12">
         <f>(1-L15)*100</f>
-        <v>-59.17460317460317</v>
+        <v>-11.422222222222222</v>
       </c>
       <c r="P15">
         <f>P14*100</f>
@@ -782,7 +782,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="2">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>13</v>
@@ -792,11 +792,11 @@
       </c>
       <c r="L16" s="13">
         <f t="shared" ref="L16:L17" si="0">K16/H16</f>
-        <v>1.7164237288135593</v>
+        <v>0.63293125000000006</v>
       </c>
       <c r="M16" s="12">
         <f t="shared" ref="M16:M17" si="1">(1-L16)*100</f>
-        <v>-71.642372881355925</v>
+        <v>36.706874999999997</v>
       </c>
     </row>
     <row r="17" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -804,7 +804,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="2">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>22</v>
@@ -812,13 +812,13 @@
       <c r="K17" s="1">
         <v>90.09</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="M17" s="12">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>1.0000000000000009</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
       </c>
       <c r="H19" s="10">
         <f>SQRT(H15*H15+H16*H16)</f>
-        <v>86.313382508160345</v>
+        <v>183.5755975068582</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>13</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="H20" s="11">
         <f>ATAN2(H15,H16)</f>
-        <v>0.75262301899337258</v>
+        <v>1.0584068664841588</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>21</v>
@@ -852,7 +852,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="10">
         <f>DEGREES(H20)</f>
-        <v>43.122122552714643</v>
+        <v>60.642246457208728</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>22</v>
@@ -867,7 +867,7 @@
       </c>
       <c r="H23" s="10">
         <f>H17-H21</f>
-        <v>47.877877447285357</v>
+        <v>-60.642246457208728</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Asser polaire mise en place + trajectoire trapez pour la vitesse + actuellement entrein de déterminer les bon coeff
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7CF3F0-1B76-45A0-B2DF-1B15E9650236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732B9C0E-FB7B-40DD-979F-1A8ED4749CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -144,6 +144,24 @@
   </si>
   <si>
     <t>Consigne droite cc</t>
+  </si>
+  <si>
+    <t>Dacc</t>
+  </si>
+  <si>
+    <t>Dcroi</t>
+  </si>
+  <si>
+    <t>Dcc</t>
+  </si>
+  <si>
+    <t>Hyp</t>
+  </si>
+  <si>
+    <t>Hyp act</t>
+  </si>
+  <si>
+    <t>Dist parc</t>
   </si>
 </sst>
 </file>
@@ -550,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,7 +817,7 @@
         <v>36.706874999999997</v>
       </c>
     </row>
-    <row r="17" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G17" s="9" t="s">
         <v>18</v>
       </c>
@@ -821,10 +839,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G19" s="4" t="s">
         <v>19</v>
       </c>
@@ -836,7 +854,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G20" s="4" t="s">
         <v>20</v>
       </c>
@@ -848,7 +866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G21" s="8"/>
       <c r="H21" s="10">
         <f>DEGREES(H20)</f>
@@ -858,10 +876,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22">
+        <v>300</v>
+      </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="7:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23">
+        <f>$B$22*1/3</f>
+        <v>100</v>
+      </c>
       <c r="G23" s="4" t="s">
         <v>23</v>
       </c>
@@ -873,8 +904,25 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="7:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:B25" si="2">$B$22*1/3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
         <v>31</v>
       </c>
@@ -882,7 +930,13 @@
         <v>59.5</v>
       </c>
     </row>
-    <row r="27" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>300</v>
+      </c>
       <c r="G27" t="s">
         <v>32</v>
       </c>
@@ -890,7 +944,14 @@
         <v>-60</v>
       </c>
     </row>
-    <row r="28" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <f>B27-B23</f>
+        <v>200</v>
+      </c>
       <c r="G28" t="s">
         <v>33</v>
       </c>
@@ -899,7 +960,7 @@
         <v>59.75</v>
       </c>
     </row>
-    <row r="29" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G29" t="s">
         <v>34</v>
       </c>
@@ -908,7 +969,7 @@
         <v>59.75</v>
       </c>
     </row>
-    <row r="30" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
J'ai trouvé les bon coeff, et effectuer un modification sur la maniere de calculer l'angle + Lecture sur le can des infos envoyé par la batterie par la carte de la base roulante + nouvelle implémentation de la carte maitre esp32 qui maintenant peut envoyé les commandes d'ouverture et de fermetture des interrupteur sur le can + Bug du wifi de l'esp 32 maitre pour une raison inconnue + Sur l'esp32 avec la bibliotheque twai pour le can, il faut mettre le if pour éviter d'essayer d'envoyé un message alors que le buffer est plein
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732B9C0E-FB7B-40DD-979F-1A8ED4749CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7E43FE-C833-400F-8C62-CCC3E645F3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -162,6 +163,48 @@
   </si>
   <si>
     <t>Dist parc</t>
+  </si>
+  <si>
+    <t>X voulue</t>
+  </si>
+  <si>
+    <t>Y voulue</t>
+  </si>
+  <si>
+    <t>X actuel</t>
+  </si>
+  <si>
+    <t>Y actuel</t>
+  </si>
+  <si>
+    <t>Theta a parcourir</t>
+  </si>
+  <si>
+    <t>X au carré</t>
+  </si>
+  <si>
+    <t>Y au carré</t>
+  </si>
+  <si>
+    <t>Tetha actuel</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theta </t>
+  </si>
+  <si>
+    <t>degres</t>
+  </si>
+  <si>
+    <t>J'obtiens expérimentalement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour une consigne de coordonnée suivante : </t>
   </si>
 </sst>
 </file>
@@ -253,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +329,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,6 +347,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>718617</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>150520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96DFC17F-AA9D-DB77-0CAB-2187400BACF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1432560"/>
+          <a:ext cx="3096057" cy="181000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>737670</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>51471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2D2DEC3-F21F-18CB-F50E-9C9E801BC154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1805940"/>
+          <a:ext cx="3115110" cy="257211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>680512</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>7647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D14B773-095A-C97F-639B-AD5C56145593}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2194560"/>
+          <a:ext cx="3057952" cy="190527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>32424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9591058-0224-868B-6403-6881488A0F99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2499360"/>
+          <a:ext cx="3191320" cy="276264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -566,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,6 +1102,12 @@
       <c r="I21" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="K21" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21">
+        <v>200</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -884,6 +1117,12 @@
         <v>300</v>
       </c>
       <c r="I22" s="1"/>
+      <c r="K22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22">
+        <v>200</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -903,6 +1142,12 @@
       <c r="I23" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="K23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23">
+        <v>182</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -912,6 +1157,12 @@
         <f t="shared" ref="B24:B25" si="2">$B$22*1/3</f>
         <v>100</v>
       </c>
+      <c r="K24" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24">
+        <v>188.6</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -921,6 +1172,13 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
+      <c r="K25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L25">
+        <f>(L21-L23)^2</f>
+        <v>324</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
@@ -929,6 +1187,13 @@
       <c r="H26">
         <v>59.5</v>
       </c>
+      <c r="K26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L26">
+        <f>(L22-L24)^2</f>
+        <v>129.96000000000012</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -943,6 +1208,12 @@
       <c r="H27">
         <v>-60</v>
       </c>
+      <c r="K27" t="s">
+        <v>49</v>
+      </c>
+      <c r="L27">
+        <v>45</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -968,6 +1239,13 @@
         <f>H28</f>
         <v>59.75</v>
       </c>
+      <c r="K29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29">
+        <f>SQRT($L$25+$L$26)</f>
+        <v>21.306337085477647</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
@@ -977,8 +1255,95 @@
         <f>-H28</f>
         <v>-59.75</v>
       </c>
+      <c r="K30" t="s">
+        <v>46</v>
+      </c>
+      <c r="L30">
+        <f>ATAN2($L$25,$L$26)</f>
+        <v>0.38146386437242458</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <f>DEGREES(L30)-L27</f>
+        <v>-23.143730534709221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K32" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32">
+        <f>ATAN2($L$26,$L$25)</f>
+        <v>1.1893324624224719</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <f>DEGREES(L32)-L27</f>
+        <v>23.143730534709221</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDAA7C3-1C16-46CF-91F2-0BA39539FEFD}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
J'ai retirer la machine a etat permettant de faire le profil trapezoidal et j'ai essayer de faire fonctionner l'asser polaire tick mais ca fonctionne presque, il faut encore jouer avec les coeff
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7E43FE-C833-400F-8C62-CCC3E645F3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEFD024-56F7-4263-9B76-812C356C4169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView topLeftCell="G19" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="G12" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDAA7C3-1C16-46CF-91F2-0BA39539FEFD}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Errer dist avec déceleration, faut faire pareil avec l'orient. Implémentation du code On/off interrupteur batterie + restart via liaison séri
</commit_message>
<xml_diff>
--- a/CodeBaseRoulanteOTA/Calcul divers.xlsx
+++ b/CodeBaseRoulanteOTA/Calcul divers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkat\Documents\PlatformIO\Projects\Enfin\CRAC-TEAM-PERSONNAL\CodeBaseRoulanteOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEFD024-56F7-4263-9B76-812C356C4169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B1629C-229F-4CAD-8DFB-9534112D4E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t xml:space="preserve">Consigne </t>
   </si>
@@ -165,46 +165,55 @@
     <t>Dist parc</t>
   </si>
   <si>
-    <t>X voulue</t>
-  </si>
-  <si>
-    <t>Y voulue</t>
-  </si>
-  <si>
-    <t>X actuel</t>
-  </si>
-  <si>
-    <t>Y actuel</t>
-  </si>
-  <si>
-    <t>Theta a parcourir</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theta </t>
+  </si>
+  <si>
+    <t>degres</t>
+  </si>
+  <si>
+    <t>J'obtiens expérimentalement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour une consigne de coordonnée suivante : </t>
+  </si>
+  <si>
+    <t>x cons</t>
+  </si>
+  <si>
+    <t>y cons</t>
+  </si>
+  <si>
+    <t>x actu</t>
+  </si>
+  <si>
+    <t>x cons - x actu</t>
+  </si>
+  <si>
+    <t>y cons - y actu</t>
+  </si>
+  <si>
+    <t>theta robot</t>
+  </si>
+  <si>
+    <t>erreur orient</t>
+  </si>
+  <si>
+    <t>y act</t>
   </si>
   <si>
     <t>X au carré</t>
   </si>
   <si>
-    <t>Y au carré</t>
-  </si>
-  <si>
-    <t>Tetha actuel</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theta </t>
-  </si>
-  <si>
-    <t>degres</t>
-  </si>
-  <si>
-    <t>J'obtiens expérimentalement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pour une consigne de coordonnée suivante : </t>
+    <t>y au carré</t>
+  </si>
+  <si>
+    <t>Erreur dist</t>
   </si>
 </sst>
 </file>
@@ -793,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G12" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="G41" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,12 +1111,6 @@
       <c r="I21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K21" t="s">
-        <v>42</v>
-      </c>
-      <c r="L21">
-        <v>200</v>
-      </c>
     </row>
     <row r="22" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -1117,12 +1120,6 @@
         <v>300</v>
       </c>
       <c r="I22" s="1"/>
-      <c r="K22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L22">
-        <v>200</v>
-      </c>
     </row>
     <row r="23" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -1142,12 +1139,6 @@
       <c r="I23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K23" t="s">
-        <v>44</v>
-      </c>
-      <c r="L23">
-        <v>182</v>
-      </c>
     </row>
     <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1157,12 +1148,6 @@
         <f t="shared" ref="B24:B25" si="2">$B$22*1/3</f>
         <v>100</v>
       </c>
-      <c r="K24" t="s">
-        <v>45</v>
-      </c>
-      <c r="L24">
-        <v>188.6</v>
-      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1172,13 +1157,6 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="K25" t="s">
-        <v>47</v>
-      </c>
-      <c r="L25">
-        <f>(L21-L23)^2</f>
-        <v>324</v>
-      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
@@ -1187,13 +1165,6 @@
       <c r="H26">
         <v>59.5</v>
       </c>
-      <c r="K26" t="s">
-        <v>48</v>
-      </c>
-      <c r="L26">
-        <f>(L22-L24)^2</f>
-        <v>129.96000000000012</v>
-      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1208,12 +1179,6 @@
       <c r="H27">
         <v>-60</v>
       </c>
-      <c r="K27" t="s">
-        <v>49</v>
-      </c>
-      <c r="L27">
-        <v>45</v>
-      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1239,13 +1204,6 @@
         <f>H28</f>
         <v>59.75</v>
       </c>
-      <c r="K29" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29">
-        <f>SQRT($L$25+$L$26)</f>
-        <v>21.306337085477647</v>
-      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
@@ -1255,33 +1213,123 @@
         <f>-H28</f>
         <v>-59.75</v>
       </c>
-      <c r="K30" t="s">
-        <v>46</v>
-      </c>
-      <c r="L30">
-        <f>ATAN2($L$25,$L$26)</f>
-        <v>0.38146386437242458</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L31">
-        <f>DEGREES(L30)-L27</f>
-        <v>-23.143730534709221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K32" t="s">
-        <v>46</v>
-      </c>
-      <c r="L32">
-        <f>ATAN2($L$26,$L$25)</f>
-        <v>1.1893324624224719</v>
-      </c>
-    </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L33">
-        <f>DEGREES(L32)-L27</f>
-        <v>23.143730534709221</v>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41">
+        <f>H36-H38</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42">
+        <f>H37-H39</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>56</v>
+      </c>
+      <c r="H44">
+        <f>H41*H41</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>57</v>
+      </c>
+      <c r="H45">
+        <f>H42*H42</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="46" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>58</v>
+      </c>
+      <c r="H46">
+        <f>SQRT(H44+H45)</f>
+        <v>141.42135623730951</v>
+      </c>
+    </row>
+    <row r="48" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48">
+        <v>-1.0389999999999999</v>
+      </c>
+      <c r="I48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H49">
+        <f>RADIANS(H48)</f>
+        <v>-1.8133970928221083E-2</v>
+      </c>
+      <c r="I49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>54</v>
+      </c>
+      <c r="H50">
+        <f>ATAN2(H41,H42)-H49</f>
+        <v>0.80353213432566939</v>
+      </c>
+      <c r="I50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H51">
+        <f>DEGREES(H50)</f>
+        <v>46.039000000000001</v>
+      </c>
+      <c r="I51" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1301,12 +1349,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -1317,7 +1365,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -1328,18 +1376,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>45</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>